<commit_message>
#remove static dynamic excel read
</commit_message>
<xml_diff>
--- a/OnlyTestingProject/Datautils/DataTestNG.xlsx
+++ b/OnlyTestingProject/Datautils/DataTestNG.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="14835" windowHeight="6375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,12 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Ankit</t>
   </si>
@@ -31,6 +32,9 @@
   </si>
   <si>
     <t>Dert</t>
+  </si>
+  <si>
+    <t>567abc</t>
   </si>
 </sst>
 </file>
@@ -364,9 +368,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
@@ -377,8 +379,8 @@
       <c r="B1">
         <v>200</v>
       </c>
-      <c r="C1">
-        <v>567</v>
+      <c r="C1" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">

</xml_diff>